<commit_message>
Documentation - attempt to correct scenarios
</commit_message>
<xml_diff>
--- a/documentation/Scenare/Scenare_stavy.xlsx
+++ b/documentation/Scenare/Scenare_stavy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="7755"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>UC3</t>
   </si>
@@ -27,9 +27,6 @@
     <t>S2</t>
   </si>
   <si>
-    <t>Editace vytvořené pizzy + aktivace/deaktivace</t>
-  </si>
-  <si>
     <t>UC2</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Připraveno k implementaci</t>
   </si>
   <si>
-    <t>Implementována alfa verze</t>
-  </si>
-  <si>
     <t>Implementace schválena zákazníkem</t>
   </si>
   <si>
@@ -175,6 +169,18 @@
   </si>
   <si>
     <t>13.12. - 20.12.</t>
+  </si>
+  <si>
+    <t>Editace vytvořené pizzy, deaktivace</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>Implementace ukončena</t>
+  </si>
+  <si>
+    <t>Implementována započata</t>
   </si>
 </sst>
 </file>
@@ -225,7 +231,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +262,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -556,9 +568,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -631,9 +640,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -651,6 +657,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1004,595 +1016,600 @@
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="25"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="7"/>
       <c r="P2" s="8"/>
     </row>
     <row r="3" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="27"/>
+        <v>53</v>
+      </c>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="40"/>
+    </row>
+    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+      <c r="E7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="18"/>
+    </row>
+    <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+      <c r="E8" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="19"/>
-    </row>
-    <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-      <c r="E7" s="38" t="s">
+      <c r="G8" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="H8" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="J8" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="L8" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="39" t="s">
+      <c r="M8" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="39" t="s">
+      <c r="N8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="O8" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="P8" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="O7" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" s="41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="11" t="str">
-        <f t="shared" ref="C8:C25" si="0">CONCATENATE(A8,B8)</f>
-        <v>UC1S1</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="37"/>
     </row>
     <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="str">
+        <f t="shared" ref="C9:C26" si="0">CONCATENATE(A9,B9)</f>
+        <v>UC1S1</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="35"/>
+    </row>
+    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="str">
+      <c r="C10" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC1S2</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12" t="str">
+      <c r="D10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC2S1</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="20"/>
+    </row>
+    <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="12" t="str">
+      <c r="C12" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC2S2</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="D12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>UC2S3</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="21"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="20"/>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12" t="str">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>UC3S1</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="21"/>
+        <v>UC2S3</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="12" t="str">
+        <v>4</v>
+      </c>
+      <c r="C14" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>UC3S2</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+        <v>UC3S1</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="30"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="21"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="20"/>
     </row>
     <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>UC3S3</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="20"/>
+        <v>UC3S2</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="19"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="25"/>
+      <c r="K15" s="29"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="21"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="20"/>
     </row>
     <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="12" t="str">
+        <v>11</v>
+      </c>
+      <c r="C16" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>UC4S1</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="20"/>
+        <v>UC3S3</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="19"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="21"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="20"/>
     </row>
     <row r="17" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>UC4S1</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="20"/>
+    </row>
+    <row r="18" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="12" t="str">
+      <c r="C18" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC4S2</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="21"/>
-    </row>
-    <row r="18" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="12" t="str">
+      <c r="D18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="20"/>
+    </row>
+    <row r="19" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC4S3</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="21"/>
-    </row>
-    <row r="19" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="12" t="str">
+      <c r="D19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="20"/>
+    </row>
+    <row r="20" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC5S1</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="21"/>
-    </row>
-    <row r="20" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="D20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="E20" s="19"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="20"/>
+    </row>
+    <row r="21" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="12" t="str">
+      <c r="C21" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC5S2</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="21"/>
-    </row>
-    <row r="21" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>UC6S1</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="20"/>
+      <c r="D21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="19"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="21"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="20"/>
     </row>
     <row r="22" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="12" t="str">
+        <v>4</v>
+      </c>
+      <c r="C22" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>UC6S2</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="20"/>
+        <v>UC6S1</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="19"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="30"/>
+      <c r="K22" s="29"/>
       <c r="L22" s="9"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="21"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="20"/>
     </row>
     <row r="23" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="C23" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>UC6S2</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="20"/>
+    </row>
+    <row r="24" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC7S1</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="21"/>
-    </row>
-    <row r="24" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="D24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="20"/>
+    </row>
+    <row r="25" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="12" t="str">
+      <c r="C25" s="11" t="str">
         <f t="shared" si="0"/>
         <v>UC7S2</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="21"/>
-    </row>
-    <row r="25" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="13" t="str">
+      <c r="D25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="20"/>
+    </row>
+    <row r="26" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="12" t="str">
         <f t="shared" si="0"/>
         <v>UC7S3</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="24"/>
-    </row>
-    <row r="26" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="3"/>
+      <c r="D26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="23"/>
     </row>
     <row r="27" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="4"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
@@ -1602,6 +1619,9 @@
     </row>
     <row r="30" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A2:E19">

</xml_diff>

<commit_message>
Documentation - add 4 more scenarios
</commit_message>
<xml_diff>
--- a/documentation/Scenare/Scenare_stavy.xlsx
+++ b/documentation/Scenare/Scenare_stavy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="7755"/>
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1170,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="29"/>
-      <c r="L10" s="9"/>
+      <c r="L10" s="24"/>
       <c r="M10" s="29"/>
       <c r="N10" s="29"/>
       <c r="O10" s="29"/>
@@ -1359,7 +1359,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="29"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="24"/>
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="29"/>
@@ -1413,7 +1413,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="29"/>
-      <c r="L19" s="9"/>
+      <c r="L19" s="24"/>
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
       <c r="O19" s="29"/>
@@ -1602,7 +1602,7 @@
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
       <c r="K26" s="31"/>
-      <c r="L26" s="22"/>
+      <c r="L26" s="24"/>
       <c r="M26" s="31"/>
       <c r="N26" s="31"/>
       <c r="O26" s="31"/>

</xml_diff>

<commit_message>
Documentation - update scenarios
</commit_message>
<xml_diff>
--- a/documentation/Scenare/Scenare_stavy.xlsx
+++ b/documentation/Scenare/Scenare_stavy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>UC3</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Implementována započata</t>
+  </si>
+  <si>
+    <t>E5</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1005,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1081,9 @@
       <c r="L7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="28"/>
+      <c r="M7" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
       <c r="P7" s="18"/>
@@ -1144,7 +1149,7 @@
       <c r="J9" s="33"/>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
+      <c r="M9" s="33"/>
       <c r="N9" s="34"/>
       <c r="O9" s="34"/>
       <c r="P9" s="35"/>
@@ -1171,7 +1176,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="29"/>
       <c r="L10" s="24"/>
-      <c r="M10" s="29"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="29"/>
       <c r="O10" s="29"/>
       <c r="P10" s="20"/>
@@ -1198,7 +1203,7 @@
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="29"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
       <c r="P11" s="20"/>
@@ -1225,7 +1230,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
-      <c r="M12" s="29"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="29"/>
       <c r="O12" s="29"/>
       <c r="P12" s="20"/>
@@ -1252,7 +1257,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
-      <c r="M13" s="29"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="29"/>
       <c r="O13" s="29"/>
       <c r="P13" s="20"/>
@@ -1279,7 +1284,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
-      <c r="M14" s="29"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="29"/>
       <c r="O14" s="29"/>
       <c r="P14" s="20"/>
@@ -1306,7 +1311,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="29"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="29"/>
+      <c r="M15" s="24"/>
       <c r="N15" s="29"/>
       <c r="O15" s="29"/>
       <c r="P15" s="20"/>
@@ -1332,8 +1337,8 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="29"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="29"/>
       <c r="O16" s="29"/>
       <c r="P16" s="20"/>
@@ -1360,7 +1365,7 @@
       <c r="J17" s="9"/>
       <c r="K17" s="29"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="29"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="29"/>
       <c r="O17" s="29"/>
       <c r="P17" s="20"/>
@@ -1387,7 +1392,7 @@
       <c r="J18" s="24"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
-      <c r="M18" s="29"/>
+      <c r="M18" s="24"/>
       <c r="N18" s="29"/>
       <c r="O18" s="29"/>
       <c r="P18" s="20"/>
@@ -1414,7 +1419,7 @@
       <c r="J19" s="9"/>
       <c r="K19" s="29"/>
       <c r="L19" s="24"/>
-      <c r="M19" s="29"/>
+      <c r="M19" s="24"/>
       <c r="N19" s="29"/>
       <c r="O19" s="29"/>
       <c r="P19" s="20"/>
@@ -1441,7 +1446,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
-      <c r="M20" s="29"/>
+      <c r="M20" s="41"/>
       <c r="N20" s="29"/>
       <c r="O20" s="29"/>
       <c r="P20" s="20"/>
@@ -1468,7 +1473,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
-      <c r="M21" s="29"/>
+      <c r="M21" s="24"/>
       <c r="N21" s="29"/>
       <c r="O21" s="29"/>
       <c r="P21" s="20"/>
@@ -1495,7 +1500,7 @@
       <c r="J22" s="9"/>
       <c r="K22" s="29"/>
       <c r="L22" s="9"/>
-      <c r="M22" s="29"/>
+      <c r="M22" s="24"/>
       <c r="N22" s="29"/>
       <c r="O22" s="29"/>
       <c r="P22" s="20"/>
@@ -1522,7 +1527,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="29"/>
       <c r="L23" s="9"/>
-      <c r="M23" s="29"/>
+      <c r="M23" s="24"/>
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
       <c r="P23" s="20"/>
@@ -1549,7 +1554,7 @@
       <c r="J24" s="41"/>
       <c r="K24" s="41"/>
       <c r="L24" s="41"/>
-      <c r="M24" s="29"/>
+      <c r="M24" s="41"/>
       <c r="N24" s="29"/>
       <c r="O24" s="29"/>
       <c r="P24" s="20"/>
@@ -1576,7 +1581,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="24"/>
       <c r="L25" s="30"/>
-      <c r="M25" s="29"/>
+      <c r="M25" s="30"/>
       <c r="N25" s="29"/>
       <c r="O25" s="29"/>
       <c r="P25" s="20"/>
@@ -1603,7 +1608,7 @@
       <c r="J26" s="22"/>
       <c r="K26" s="31"/>
       <c r="L26" s="24"/>
-      <c r="M26" s="31"/>
+      <c r="M26" s="24"/>
       <c r="N26" s="31"/>
       <c r="O26" s="31"/>
       <c r="P26" s="23"/>

</xml_diff>

<commit_message>
Documentation - update scenario states
Documentation - update scenario states
</commit_message>
<xml_diff>
--- a/documentation/Scenare/Scenare_stavy.xlsx
+++ b/documentation/Scenare/Scenare_stavy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>UC3</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
   </si>
 </sst>
 </file>
@@ -272,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -513,6 +522,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -520,22 +555,20 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -601,18 +634,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -628,43 +655,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1005,7 +1038,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1057,7 @@
       <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="23"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,13 +1071,13 @@
       <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
@@ -1075,55 +1108,61 @@
       <c r="J7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="26" t="s">
         <v>33</v>
       </c>
       <c r="L7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="18"/>
+      <c r="N7" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="38" t="s">
+      <c r="O8" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="39" t="s">
+      <c r="P8" s="40" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1141,18 +1180,18 @@
       <c r="D9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="35"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="31"/>
     </row>
     <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1174,12 +1213,12 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="20"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="32"/>
     </row>
     <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1196,17 +1235,17 @@
         <v>10</v>
       </c>
       <c r="E11" s="19"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="33"/>
     </row>
     <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1228,12 +1267,12 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="20"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="32"/>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1255,12 +1294,12 @@
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="20"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="32"/>
     </row>
     <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1277,17 +1316,17 @@
         <v>5</v>
       </c>
       <c r="E14" s="19"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="20"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="34"/>
     </row>
     <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1309,12 +1348,12 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="29"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="20"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="34"/>
     </row>
     <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1336,12 +1375,12 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="20"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="34"/>
     </row>
     <row r="17" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1363,12 +1402,12 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="20"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="32"/>
     </row>
     <row r="18" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1385,17 +1424,17 @@
         <v>14</v>
       </c>
       <c r="E18" s="19"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="20"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="32"/>
     </row>
     <row r="19" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1417,12 +1456,12 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="20"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="32"/>
     </row>
     <row r="20" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1439,17 +1478,17 @@
         <v>22</v>
       </c>
       <c r="E20" s="19"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="20"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="34"/>
     </row>
     <row r="21" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -1471,12 +1510,12 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="20"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="32"/>
     </row>
     <row r="22" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1498,12 +1537,12 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="29"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="9"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="20"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="32"/>
     </row>
     <row r="23" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1525,12 +1564,12 @@
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="29"/>
+      <c r="K23" s="9"/>
       <c r="L23" s="9"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="20"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="32"/>
     </row>
     <row r="24" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
@@ -1547,17 +1586,17 @@
         <v>17</v>
       </c>
       <c r="E24" s="19"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="20"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="34"/>
     </row>
     <row r="25" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -1579,12 +1618,12 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="20"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="33"/>
     </row>
     <row r="26" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
@@ -1600,18 +1639,18 @@
       <c r="D26" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="23"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="36"/>
     </row>
     <row r="27" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>

</xml_diff>